<commit_message>
Creating database connections, data sources and data models, to interact with the database.
</commit_message>
<xml_diff>
--- a/docs/database_desing.xlsx
+++ b/docs/database_desing.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>text</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>Flags to know the app status ( 0 normal, 1 Installing, 2 Updating, 3 Desinstallig), this flags will be used to determinate the functionality of the activitys, menus and mesagges</t>
+  </si>
+  <si>
+    <t>edited</t>
+  </si>
+  <si>
+    <t>timestamp of the edition date</t>
   </si>
 </sst>
 </file>
@@ -139,7 +145,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -171,11 +177,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -186,11 +203,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -469,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -481,12 +504,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -586,31 +609,45 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="96" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>